<commit_message>
fix tests, move tests
</commit_message>
<xml_diff>
--- a/Regression/templates/Product_Configs_Provar.xlsx
+++ b/Regression/templates/Product_Configs_Provar.xlsx
@@ -1085,9 +1085,6 @@
     <t>VehicleSorting</t>
   </si>
   <si>
-    <t>ArtworkPreApproveCase#</t>
-  </si>
-  <si>
     <t>FrontLineProModel</t>
   </si>
   <si>
@@ -1299,6 +1296,9 @@
   </si>
   <si>
     <t>o</t>
+  </si>
+  <si>
+    <t>ArtworkPreApproveCaseNo</t>
   </si>
 </sst>
 </file>
@@ -2943,8 +2943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:JC128"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="FB1" workbookViewId="0">
-      <selection activeCell="FJ1" sqref="FJ1:FQ1048576"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="IE79" workbookViewId="0">
+      <selection activeCell="IG88" sqref="IG88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3169,7 +3169,7 @@
   <sheetData>
     <row r="1" spans="1:263" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>169</v>
@@ -3193,22 +3193,22 @@
         <v>137</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>355</v>
+        <v>426</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>173</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>370</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>371</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>174</v>
@@ -3217,7 +3217,7 @@
         <v>175</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>176</v>
@@ -3229,7 +3229,7 @@
         <v>178</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>179</v>
@@ -3238,7 +3238,7 @@
         <v>180</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="Y1" s="2" t="s">
         <v>181</v>
@@ -3247,10 +3247,10 @@
         <v>182</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AB1" s="2" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="AC1" s="2" t="s">
         <v>1</v>
@@ -3292,10 +3292,10 @@
         <v>193</v>
       </c>
       <c r="AP1" s="2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="AQ1" s="2" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AR1" s="2" t="s">
         <v>194</v>
@@ -3304,7 +3304,7 @@
         <v>195</v>
       </c>
       <c r="AT1" s="2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="AU1" s="2" t="s">
         <v>196</v>
@@ -3322,19 +3322,19 @@
         <v>200</v>
       </c>
       <c r="AZ1" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="BA1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="BB1" s="2" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="BC1" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="BD1" s="2" t="s">
         <v>375</v>
-      </c>
-      <c r="BD1" s="2" t="s">
-        <v>376</v>
       </c>
       <c r="BE1" s="2" t="s">
         <v>201</v>
@@ -3394,25 +3394,25 @@
         <v>219</v>
       </c>
       <c r="BX1" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="BY1" s="2" t="s">
         <v>220</v>
       </c>
       <c r="BZ1" s="2" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="CA1" s="2" t="s">
         <v>221</v>
       </c>
       <c r="CB1" s="2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="CC1" s="2" t="s">
         <v>222</v>
       </c>
       <c r="CD1" s="2" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="CE1" s="2" t="s">
         <v>223</v>
@@ -3421,7 +3421,7 @@
         <v>224</v>
       </c>
       <c r="CG1" s="2" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="CH1" s="2" t="s">
         <v>225</v>
@@ -3439,7 +3439,7 @@
         <v>229</v>
       </c>
       <c r="CM1" s="2" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="CN1" s="2" t="s">
         <v>230</v>
@@ -3463,25 +3463,25 @@
         <v>236</v>
       </c>
       <c r="CU1" s="2" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="CV1" s="2" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="CW1" s="2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="CX1" s="2" t="s">
         <v>237</v>
       </c>
       <c r="CY1" s="2" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="CZ1" s="2" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="DA1" s="2" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="DB1" s="2" t="s">
         <v>4</v>
@@ -3490,10 +3490,10 @@
         <v>238</v>
       </c>
       <c r="DD1" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="DE1" s="2" t="s">
         <v>372</v>
-      </c>
-      <c r="DE1" s="2" t="s">
-        <v>373</v>
       </c>
       <c r="DF1" s="2" t="s">
         <v>239</v>
@@ -3508,7 +3508,7 @@
         <v>241</v>
       </c>
       <c r="DJ1" s="2" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="DK1" s="2" t="s">
         <v>242</v>
@@ -3520,7 +3520,7 @@
         <v>244</v>
       </c>
       <c r="DN1" s="2" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="DO1" s="2" t="s">
         <v>245</v>
@@ -3532,7 +3532,7 @@
         <v>247</v>
       </c>
       <c r="DR1" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="DS1" s="2" t="s">
         <v>248</v>
@@ -3544,7 +3544,7 @@
         <v>250</v>
       </c>
       <c r="DV1" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="DW1" s="2" t="s">
         <v>251</v>
@@ -3664,31 +3664,31 @@
         <v>289</v>
       </c>
       <c r="FJ1" s="13" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="FK1" s="13" t="s">
+        <v>418</v>
+      </c>
+      <c r="FL1" s="13" t="s">
         <v>419</v>
       </c>
-      <c r="FL1" s="13" t="s">
+      <c r="FM1" s="13" t="s">
         <v>420</v>
       </c>
-      <c r="FM1" s="13" t="s">
+      <c r="FN1" s="13" t="s">
         <v>421</v>
       </c>
-      <c r="FN1" s="13" t="s">
+      <c r="FO1" s="13" t="s">
         <v>422</v>
       </c>
-      <c r="FO1" s="13" t="s">
+      <c r="FP1" s="13" t="s">
         <v>423</v>
       </c>
-      <c r="FP1" s="13" t="s">
+      <c r="FQ1" s="13" t="s">
         <v>424</v>
       </c>
-      <c r="FQ1" s="13" t="s">
-        <v>425</v>
-      </c>
       <c r="FR1" s="2" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="FS1" s="2" t="s">
         <v>5</v>
@@ -3697,10 +3697,10 @@
         <v>290</v>
       </c>
       <c r="FU1" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="FV1" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="FV1" s="2" t="s">
-        <v>405</v>
       </c>
       <c r="FW1" s="2" t="s">
         <v>291</v>
@@ -3730,10 +3730,10 @@
         <v>299</v>
       </c>
       <c r="GF1" s="2" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="GG1" s="2" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="GH1" s="2" t="s">
         <v>300</v>
@@ -3787,16 +3787,16 @@
         <v>316</v>
       </c>
       <c r="GY1" s="2" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="GZ1" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="HA1" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="HB1" s="2" t="s">
         <v>365</v>
-      </c>
-      <c r="HA1" s="2" t="s">
-        <v>383</v>
-      </c>
-      <c r="HB1" s="2" t="s">
-        <v>366</v>
       </c>
       <c r="HC1" s="2" t="s">
         <v>317</v>
@@ -3814,7 +3814,7 @@
         <v>321</v>
       </c>
       <c r="HH1" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="HI1" s="2" t="s">
         <v>322</v>
@@ -3829,13 +3829,13 @@
         <v>325</v>
       </c>
       <c r="HM1" s="2" t="s">
+        <v>383</v>
+      </c>
+      <c r="HN1" s="2" t="s">
         <v>384</v>
       </c>
-      <c r="HN1" s="2" t="s">
+      <c r="HO1" s="2" t="s">
         <v>385</v>
-      </c>
-      <c r="HO1" s="2" t="s">
-        <v>386</v>
       </c>
       <c r="HP1" s="13" t="s">
         <v>326</v>
@@ -3865,25 +3865,25 @@
         <v>334</v>
       </c>
       <c r="HY1" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="HZ1" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="IA1" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="IB1" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="IC1" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="ID1" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="IE1" s="2" t="s">
         <v>392</v>
-      </c>
-      <c r="HZ1" s="2" t="s">
-        <v>387</v>
-      </c>
-      <c r="IA1" s="2" t="s">
-        <v>388</v>
-      </c>
-      <c r="IB1" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="IC1" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="ID1" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="IE1" s="2" t="s">
-        <v>393</v>
       </c>
       <c r="IF1" s="2" t="s">
         <v>335</v>
@@ -3901,7 +3901,7 @@
         <v>339</v>
       </c>
       <c r="IK1" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="IL1" s="2" t="s">
         <v>340</v>
@@ -3931,10 +3931,10 @@
         <v>348</v>
       </c>
       <c r="IU1" s="2" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="IV1" s="2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="IW1" s="2" t="s">
         <v>349</v>
@@ -3968,7 +3968,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="4">
         <f t="shared" ref="F2:F33" ca="1" si="0">TODAY()</f>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -4242,7 +4242,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -4516,7 +4516,7 @@
       <c r="E4" s="3"/>
       <c r="F4" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -4790,7 +4790,7 @@
       <c r="E5" s="3"/>
       <c r="F5" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -5066,7 +5066,7 @@
       <c r="E6" s="3"/>
       <c r="F6" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
@@ -5364,7 +5364,7 @@
       <c r="E7" s="3"/>
       <c r="F7" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
@@ -5650,7 +5650,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
@@ -5946,7 +5946,7 @@
       <c r="E9" s="3"/>
       <c r="F9" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
@@ -6236,7 +6236,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
@@ -6281,7 +6281,7 @@
         <v>144</v>
       </c>
       <c r="AI10" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ10" s="3"/>
       <c r="AK10" s="3"/>
@@ -6572,7 +6572,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -6617,7 +6617,7 @@
         <v>144</v>
       </c>
       <c r="AI11" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ11" s="3"/>
       <c r="AK11" s="3"/>
@@ -6910,7 +6910,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -6955,7 +6955,7 @@
         <v>144</v>
       </c>
       <c r="AI12" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ12" s="3"/>
       <c r="AK12" s="3"/>
@@ -7248,7 +7248,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -7570,7 +7570,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -7896,7 +7896,7 @@
       <c r="E15" s="3"/>
       <c r="F15" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
@@ -8218,7 +8218,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
@@ -8273,7 +8273,7 @@
         <v>144</v>
       </c>
       <c r="AI16" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ16" s="3"/>
       <c r="AK16" s="3"/>
@@ -8618,7 +8618,7 @@
       <c r="E17" s="3"/>
       <c r="F17" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -8673,7 +8673,7 @@
         <v>144</v>
       </c>
       <c r="AI17" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ17" s="3"/>
       <c r="AK17" s="3"/>
@@ -9020,7 +9020,7 @@
       <c r="E18" s="3"/>
       <c r="F18" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -9075,7 +9075,7 @@
         <v>144</v>
       </c>
       <c r="AI18" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ18" s="3"/>
       <c r="AK18" s="3"/>
@@ -9422,7 +9422,7 @@
       <c r="E19" s="3"/>
       <c r="F19" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -9477,7 +9477,7 @@
         <v>144</v>
       </c>
       <c r="AI19" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ19" s="3"/>
       <c r="AK19" s="3"/>
@@ -9824,7 +9824,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
@@ -9879,7 +9879,7 @@
         <v>144</v>
       </c>
       <c r="AI20" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ20" s="3"/>
       <c r="AK20" s="3"/>
@@ -10226,7 +10226,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -10259,7 +10259,7 @@
         <v>144</v>
       </c>
       <c r="AI21" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ21" s="3"/>
       <c r="AK21" s="3"/>
@@ -10552,7 +10552,7 @@
       <c r="E22" s="3"/>
       <c r="F22" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -10585,7 +10585,7 @@
         <v>144</v>
       </c>
       <c r="AI22" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ22" s="3"/>
       <c r="AK22" s="3"/>
@@ -10878,7 +10878,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -11160,7 +11160,7 @@
       <c r="E24" s="3"/>
       <c r="F24" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
@@ -11434,7 +11434,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -11708,7 +11708,7 @@
       <c r="E26" s="3"/>
       <c r="F26" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
@@ -11984,7 +11984,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
@@ -12258,7 +12258,7 @@
       <c r="E28" s="3"/>
       <c r="F28" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
@@ -12570,7 +12570,7 @@
       <c r="E29" s="3"/>
       <c r="F29" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
@@ -12868,7 +12868,7 @@
       <c r="E30" s="3"/>
       <c r="F30" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -13166,7 +13166,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -13213,7 +13213,7 @@
         <v>144</v>
       </c>
       <c r="AI31" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ31" s="3"/>
       <c r="AK31" s="3"/>
@@ -13510,7 +13510,7 @@
       <c r="E32" s="3"/>
       <c r="F32" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -13557,7 +13557,7 @@
         <v>144</v>
       </c>
       <c r="AI32" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ32" s="3"/>
       <c r="AK32" s="3"/>
@@ -13854,7 +13854,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -13895,7 +13895,7 @@
         <v>144</v>
       </c>
       <c r="AI33" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ33" s="3"/>
       <c r="AK33" s="3"/>
@@ -14178,7 +14178,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="4">
         <f t="shared" ref="F34:F65" ca="1" si="1">TODAY()</f>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
@@ -14498,7 +14498,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -14822,7 +14822,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -15144,7 +15144,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
@@ -15436,7 +15436,7 @@
       <c r="E38" s="3"/>
       <c r="F38" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
@@ -15728,7 +15728,7 @@
       <c r="E39" s="3"/>
       <c r="F39" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
@@ -15775,7 +15775,7 @@
         <v>144</v>
       </c>
       <c r="AI39" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ39" s="3"/>
       <c r="AK39" s="3"/>
@@ -16076,7 +16076,7 @@
       <c r="E40" s="3"/>
       <c r="F40" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
@@ -16123,7 +16123,7 @@
         <v>144</v>
       </c>
       <c r="AI40" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ40" s="3"/>
       <c r="AK40" s="3"/>
@@ -16442,7 +16442,7 @@
       <c r="E41" s="3"/>
       <c r="F41" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
@@ -16489,7 +16489,7 @@
         <v>144</v>
       </c>
       <c r="AI41" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ41" s="3"/>
       <c r="AK41" s="3"/>
@@ -16808,7 +16808,7 @@
       <c r="E42" s="3"/>
       <c r="F42" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
@@ -16863,7 +16863,7 @@
         <v>144</v>
       </c>
       <c r="AI42" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ42" s="3"/>
       <c r="AK42" s="3"/>
@@ -17232,7 +17232,7 @@
       <c r="E43" s="3"/>
       <c r="F43" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -17526,7 +17526,7 @@
       <c r="E44" s="3"/>
       <c r="F44" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -17856,7 +17856,7 @@
       <c r="E45" s="3"/>
       <c r="F45" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -18152,7 +18152,7 @@
       <c r="E46" s="3"/>
       <c r="F46" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
@@ -18444,7 +18444,7 @@
       <c r="E47" s="3"/>
       <c r="F47" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -18481,7 +18481,7 @@
         <v>144</v>
       </c>
       <c r="AI47" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ47" s="3"/>
       <c r="AK47" s="3"/>
@@ -18750,7 +18750,7 @@
       <c r="E48" s="3"/>
       <c r="F48" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
@@ -18797,7 +18797,7 @@
         <v>144</v>
       </c>
       <c r="AI48" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ48" s="3"/>
       <c r="AK48" s="3"/>
@@ -19116,7 +19116,7 @@
       <c r="E49" s="3"/>
       <c r="F49" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
@@ -19163,7 +19163,7 @@
         <v>144</v>
       </c>
       <c r="AI49" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ49" s="3"/>
       <c r="AK49" s="3"/>
@@ -19490,7 +19490,7 @@
       <c r="E50" s="3"/>
       <c r="F50" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
@@ -19537,7 +19537,7 @@
         <v>144</v>
       </c>
       <c r="AI50" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ50" s="3"/>
       <c r="AK50" s="3"/>
@@ -19858,7 +19858,7 @@
       <c r="E51" s="3"/>
       <c r="F51" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -20154,7 +20154,7 @@
       <c r="E52" s="3"/>
       <c r="F52" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
@@ -20450,7 +20450,7 @@
       <c r="E53" s="3"/>
       <c r="F53" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G53" s="3"/>
       <c r="H53" s="3"/>
@@ -20746,7 +20746,7 @@
       <c r="E54" s="3"/>
       <c r="F54" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G54" s="3"/>
       <c r="H54" s="3"/>
@@ -21040,7 +21040,7 @@
       <c r="E55" s="3"/>
       <c r="F55" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
@@ -21316,7 +21316,7 @@
       <c r="E56" s="3"/>
       <c r="F56" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
@@ -21596,7 +21596,7 @@
       <c r="E57" s="3"/>
       <c r="F57" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
@@ -21874,7 +21874,7 @@
       <c r="E58" s="3"/>
       <c r="F58" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
@@ -22156,7 +22156,7 @@
       <c r="E59" s="3"/>
       <c r="F59" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
@@ -22444,7 +22444,7 @@
       <c r="E60" s="3"/>
       <c r="F60" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
@@ -22768,7 +22768,7 @@
       <c r="E61" s="3"/>
       <c r="F61" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
@@ -23058,7 +23058,7 @@
       <c r="E62" s="3"/>
       <c r="F62" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
@@ -23336,7 +23336,7 @@
       <c r="E63" s="3"/>
       <c r="F63" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
@@ -23620,7 +23620,7 @@
       <c r="E64" s="3"/>
       <c r="F64" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
@@ -23906,7 +23906,7 @@
       <c r="E65" s="3"/>
       <c r="F65" s="4">
         <f t="shared" ca="1" si="1"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
@@ -24188,7 +24188,7 @@
       <c r="E66" s="3"/>
       <c r="F66" s="4">
         <f t="shared" ref="F66:F96" ca="1" si="2">TODAY()</f>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
@@ -24506,7 +24506,7 @@
       <c r="E67" s="3"/>
       <c r="F67" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
@@ -24828,7 +24828,7 @@
       <c r="E68" s="3"/>
       <c r="F68" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
@@ -25154,7 +25154,7 @@
       <c r="E69" s="3"/>
       <c r="F69" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
@@ -25476,7 +25476,7 @@
       <c r="E70" s="3"/>
       <c r="F70" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
@@ -25519,7 +25519,7 @@
         <v>144</v>
       </c>
       <c r="AI70" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ70" s="3"/>
       <c r="AK70" s="3"/>
@@ -25814,7 +25814,7 @@
       <c r="E71" s="3"/>
       <c r="F71" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
@@ -25857,7 +25857,7 @@
         <v>144</v>
       </c>
       <c r="AI71" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ71" s="3"/>
       <c r="AK71" s="3"/>
@@ -26154,7 +26154,7 @@
       <c r="E72" s="3"/>
       <c r="F72" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
@@ -26474,7 +26474,7 @@
       <c r="E73" s="3"/>
       <c r="F73" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
@@ -26796,7 +26796,7 @@
       <c r="E74" s="3"/>
       <c r="F74" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
@@ -27124,7 +27124,7 @@
       <c r="E75" s="3"/>
       <c r="F75" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
@@ -27452,7 +27452,7 @@
       <c r="E76" s="3"/>
       <c r="F76" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
@@ -27774,7 +27774,7 @@
       <c r="E77" s="3"/>
       <c r="F77" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
@@ -28098,7 +28098,7 @@
       <c r="E78" s="3"/>
       <c r="F78" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
@@ -28420,7 +28420,7 @@
       <c r="E79" s="3"/>
       <c r="F79" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G79" s="3"/>
       <c r="H79" s="3"/>
@@ -28694,7 +28694,7 @@
       <c r="E80" s="3"/>
       <c r="F80" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G80" s="3"/>
       <c r="H80" s="3"/>
@@ -28968,7 +28968,7 @@
       <c r="E81" s="3"/>
       <c r="F81" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G81" s="3"/>
       <c r="H81" s="3"/>
@@ -29242,7 +29242,7 @@
       <c r="E82" s="3"/>
       <c r="F82" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G82" s="3"/>
       <c r="H82" s="3"/>
@@ -29285,7 +29285,7 @@
         <v>144</v>
       </c>
       <c r="AI82" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ82" s="3"/>
       <c r="AK82" s="3"/>
@@ -29572,7 +29572,7 @@
       <c r="E83" s="3"/>
       <c r="F83" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G83" s="3"/>
       <c r="H83" s="3"/>
@@ -29615,7 +29615,7 @@
         <v>144</v>
       </c>
       <c r="AI83" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ83" s="3"/>
       <c r="AK83" s="3"/>
@@ -29904,7 +29904,7 @@
       <c r="E84" s="3"/>
       <c r="F84" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G84" s="3"/>
       <c r="H84" s="3"/>
@@ -29947,7 +29947,7 @@
         <v>144</v>
       </c>
       <c r="AI84" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ84" s="3"/>
       <c r="AK84" s="3"/>
@@ -30236,7 +30236,7 @@
       <c r="E85" s="3"/>
       <c r="F85" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G85" s="3"/>
       <c r="H85" s="3"/>
@@ -30550,7 +30550,7 @@
       <c r="E86" s="3"/>
       <c r="F86" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G86" s="3"/>
       <c r="H86" s="3"/>
@@ -30868,7 +30868,7 @@
       <c r="E87" s="3"/>
       <c r="F87" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G87" s="3"/>
       <c r="H87" s="3"/>
@@ -31182,7 +31182,7 @@
       <c r="E88" s="3"/>
       <c r="F88" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G88" s="3"/>
       <c r="H88" s="3"/>
@@ -31223,7 +31223,7 @@
         <v>144</v>
       </c>
       <c r="AI88" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ88" s="3"/>
       <c r="AK88" s="3"/>
@@ -31464,9 +31464,7 @@
       <c r="ID88" s="3"/>
       <c r="IE88" s="3"/>
       <c r="IF88" s="3"/>
-      <c r="IG88" s="14">
-        <v>0</v>
-      </c>
+      <c r="IG88" s="14"/>
       <c r="IH88" s="3"/>
       <c r="II88" s="3"/>
       <c r="IJ88" s="3"/>
@@ -31510,7 +31508,7 @@
       <c r="E89" s="3"/>
       <c r="F89" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
@@ -31551,7 +31549,7 @@
         <v>144</v>
       </c>
       <c r="AI89" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ89" s="3"/>
       <c r="AK89" s="3"/>
@@ -31816,7 +31814,7 @@
       <c r="E90" s="3"/>
       <c r="F90" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
@@ -31857,7 +31855,7 @@
         <v>144</v>
       </c>
       <c r="AI90" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ90" s="3"/>
       <c r="AK90" s="3"/>
@@ -32152,7 +32150,7 @@
       <c r="E91" s="3"/>
       <c r="F91" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
@@ -32193,7 +32191,7 @@
         <v>144</v>
       </c>
       <c r="AI91" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ91" s="3"/>
       <c r="AK91" s="3"/>
@@ -32488,7 +32486,7 @@
       <c r="E92" s="3"/>
       <c r="F92" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
@@ -32529,7 +32527,7 @@
         <v>144</v>
       </c>
       <c r="AI92" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ92" s="3"/>
       <c r="AK92" s="3"/>
@@ -32824,7 +32822,7 @@
       <c r="E93" s="3"/>
       <c r="F93" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G93" s="3"/>
       <c r="H93" s="3"/>
@@ -32865,7 +32863,7 @@
         <v>144</v>
       </c>
       <c r="AI93" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ93" s="3"/>
       <c r="AK93" s="3"/>
@@ -33160,7 +33158,7 @@
       <c r="E94" s="3"/>
       <c r="F94" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G94" s="3"/>
       <c r="H94" s="3"/>
@@ -33436,7 +33434,7 @@
       <c r="E95" s="3"/>
       <c r="F95" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G95" s="3"/>
       <c r="H95" s="3"/>
@@ -33712,7 +33710,7 @@
       <c r="E96" s="3"/>
       <c r="F96" s="4">
         <f t="shared" ca="1" si="2"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G96" s="3"/>
       <c r="H96" s="3"/>
@@ -34257,7 +34255,7 @@
       <c r="E98" s="3"/>
       <c r="F98" s="4">
         <f ca="1">TODAY()</f>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G98" s="3"/>
       <c r="H98" s="3"/>
@@ -34802,7 +34800,7 @@
       <c r="E100" s="3"/>
       <c r="F100" s="4">
         <f t="shared" ref="F100:F128" ca="1" si="3">TODAY()</f>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G100" s="3"/>
       <c r="H100" s="3"/>
@@ -35102,7 +35100,7 @@
       <c r="E101" s="3"/>
       <c r="F101" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G101" s="3"/>
       <c r="H101" s="3"/>
@@ -35402,7 +35400,7 @@
       <c r="E102" s="3"/>
       <c r="F102" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G102" s="3"/>
       <c r="H102" s="3"/>
@@ -35702,7 +35700,7 @@
       <c r="E103" s="3"/>
       <c r="F103" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G103" s="3"/>
       <c r="H103" s="3"/>
@@ -36000,7 +35998,7 @@
       <c r="E104" s="3"/>
       <c r="F104" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G104" s="3"/>
       <c r="H104" s="3"/>
@@ -36286,7 +36284,7 @@
       <c r="E105" s="3"/>
       <c r="F105" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G105" s="3"/>
       <c r="H105" s="3"/>
@@ -36572,7 +36570,7 @@
       <c r="E106" s="3"/>
       <c r="F106" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G106" s="3"/>
       <c r="H106" s="3"/>
@@ -36860,7 +36858,7 @@
       <c r="E107" s="3"/>
       <c r="F107" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G107" s="3"/>
       <c r="H107" s="3"/>
@@ -37148,7 +37146,7 @@
       <c r="E108" s="3"/>
       <c r="F108" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G108" s="3"/>
       <c r="H108" s="3"/>
@@ -37436,7 +37434,7 @@
       <c r="E109" s="3"/>
       <c r="F109" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G109" s="3"/>
       <c r="H109" s="3"/>
@@ -37724,7 +37722,7 @@
       <c r="E110" s="3"/>
       <c r="F110" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G110" s="3"/>
       <c r="H110" s="3"/>
@@ -38010,7 +38008,7 @@
       <c r="E111" s="3"/>
       <c r="F111" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G111" s="3"/>
       <c r="H111" s="3"/>
@@ -38312,7 +38310,7 @@
       <c r="E112" s="3"/>
       <c r="F112" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G112" s="3"/>
       <c r="H112" s="3"/>
@@ -38614,7 +38612,7 @@
       <c r="E113" s="3"/>
       <c r="F113" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G113" s="3"/>
       <c r="H113" s="3"/>
@@ -38916,7 +38914,7 @@
       <c r="E114" s="3"/>
       <c r="F114" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G114" s="3"/>
       <c r="H114" s="3"/>
@@ -39218,7 +39216,7 @@
       <c r="E115" s="3"/>
       <c r="F115" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G115" s="3"/>
       <c r="H115" s="3"/>
@@ -39520,7 +39518,7 @@
       <c r="E116" s="3"/>
       <c r="F116" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G116" s="3"/>
       <c r="H116" s="3"/>
@@ -39822,7 +39820,7 @@
       <c r="E117" s="3"/>
       <c r="F117" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G117" s="3"/>
       <c r="H117" s="3"/>
@@ -40124,7 +40122,7 @@
       <c r="E118" s="3"/>
       <c r="F118" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G118" s="3"/>
       <c r="H118" s="3"/>
@@ -40426,7 +40424,7 @@
       <c r="E119" s="3"/>
       <c r="F119" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G119" s="3"/>
       <c r="H119" s="3"/>
@@ -40728,7 +40726,7 @@
       <c r="E120" s="3"/>
       <c r="F120" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G120" s="3"/>
       <c r="H120" s="3"/>
@@ -41030,7 +41028,7 @@
       <c r="E121" s="3"/>
       <c r="F121" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G121" s="3"/>
       <c r="H121" s="3"/>
@@ -41077,7 +41075,7 @@
         <v>144</v>
       </c>
       <c r="AI121" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ121" s="3"/>
       <c r="AK121" s="3"/>
@@ -41380,7 +41378,7 @@
       <c r="E122" s="3"/>
       <c r="F122" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G122" s="3"/>
       <c r="H122" s="3"/>
@@ -41427,7 +41425,7 @@
         <v>144</v>
       </c>
       <c r="AI122" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ122" s="3"/>
       <c r="AK122" s="3"/>
@@ -41730,7 +41728,7 @@
       <c r="E123" s="3"/>
       <c r="F123" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G123" s="3"/>
       <c r="H123" s="3"/>
@@ -41777,7 +41775,7 @@
         <v>144</v>
       </c>
       <c r="AI123" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AJ123" s="3"/>
       <c r="AK123" s="3"/>
@@ -42080,7 +42078,7 @@
       <c r="E124" s="3"/>
       <c r="F124" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G124" s="3"/>
       <c r="H124" s="3"/>
@@ -42354,7 +42352,7 @@
       <c r="E125" s="3"/>
       <c r="F125" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G125" s="3"/>
       <c r="H125" s="3"/>
@@ -42628,7 +42626,7 @@
       <c r="E126" s="3"/>
       <c r="F126" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G126" s="3"/>
       <c r="H126" s="3"/>
@@ -42902,7 +42900,7 @@
       <c r="E127" s="3"/>
       <c r="F127" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G127" s="3"/>
       <c r="H127" s="3"/>
@@ -43176,7 +43174,7 @@
       <c r="E128" s="3"/>
       <c r="F128" s="4">
         <f t="shared" ca="1" si="3"/>
-        <v>42551</v>
+        <v>42569</v>
       </c>
       <c r="G128" s="3"/>
       <c r="H128" s="3"/>
@@ -43456,7 +43454,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -43475,51 +43473,49 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
+        <v>396</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>397</v>
       </c>
-      <c r="B1" s="10" t="s">
-        <v>398</v>
-      </c>
       <c r="C1" s="10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I1" s="11" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="J1" s="11" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="K1" s="11" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="10" t="s">
-        <v>28</v>
-      </c>
+      <c r="B2" s="10"/>
       <c r="C2" s="10" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E2" s="10" t="s">
         <v>68</v>
@@ -43545,12 +43541,14 @@
       <c r="A3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="10"/>
+      <c r="B3" s="10" t="s">
+        <v>28</v>
+      </c>
       <c r="C3" s="10" t="s">
         <v>43</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>22</v>

</xml_diff>